<commit_message>
added new testing file & changes to logic
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NemanjaSimpraga\Documents\cutting_scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45183292-113D-43BB-A0E5-9BE3FAB9E0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33C6F7-335B-4DB3-ADBB-35E315E8FA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4898FC76-975B-4242-BB8F-A76D91429865}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
i went too far...
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NemanjaSimpraga\Documents\cutting_scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesho\Documents\cutting_scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A33C6F7-335B-4DB3-ADBB-35E315E8FA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A961A0-A1A0-4B21-B563-0ABCC695169B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4898FC76-975B-4242-BB8F-A76D91429865}"/>
+    <workbookView xWindow="28680" yWindow="-6390" windowWidth="16440" windowHeight="28440" xr2:uid="{4898FC76-975B-4242-BB8F-A76D91429865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Group</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>SUM</t>
-  </si>
-  <si>
-    <t>OVER LIMIT</t>
   </si>
   <si>
     <t>to cut</t>
@@ -453,23 +450,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5293D0-8D68-4052-9E07-2020BCCAE873}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="H1" t="s">
         <v>3</v>
       </c>
@@ -485,23 +487,8 @@
       <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="G2" t="s">
         <v>8</v>
       </c>
@@ -521,47 +508,47 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3">
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3">
+        <v>70</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>365</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="D3">
-        <v>0.28571428999999998</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3">
-        <v>80</v>
-      </c>
-      <c r="I3">
-        <v>120</v>
-      </c>
-      <c r="J3">
-        <v>70</v>
-      </c>
-      <c r="K3">
-        <v>20</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>375</v>
-      </c>
-      <c r="C4">
-        <v>5.0999999999999996</v>
       </c>
       <c r="D4">
         <v>0.28571428999999998</v>
@@ -570,72 +557,72 @@
         <v>10</v>
       </c>
       <c r="H4">
-        <f>$H$3*D3*B3</f>
+        <f>$H$3*D4*B4</f>
+        <v>4692.8572132499994</v>
+      </c>
+      <c r="I4">
+        <f>$I$3*D4*B4</f>
+        <v>7300.0001094999998</v>
+      </c>
+      <c r="J4">
+        <f>$J$3*D4*B4</f>
+        <v>2085.7143169999999</v>
+      </c>
+      <c r="K4">
+        <f>$K$3*D4*B4</f>
+        <v>10428.571585</v>
+      </c>
+      <c r="L4">
+        <f>$L$3*D4*B4</f>
         <v>8342.8572679999997</v>
       </c>
-      <c r="I4">
-        <f>$I$3*D3*B3</f>
-        <v>12514.285902</v>
-      </c>
-      <c r="J4">
-        <f>$J$3*D3*B3</f>
-        <v>7300.0001094999998</v>
-      </c>
-      <c r="K4">
-        <f>$K$3*D3*B3</f>
-        <v>2085.7143169999999</v>
-      </c>
-      <c r="L4">
-        <f>$L$3*D3*B3</f>
-        <v>10428.571585</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D5">
-        <v>0.14285713999999999</v>
+        <v>0.28571428999999998</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H8" si="0">$H$3*D4*B4</f>
+        <f>$H$3*D5*B5</f>
+        <v>4821.4286437499995</v>
+      </c>
+      <c r="I5">
+        <f>$I$3*D5*B5</f>
+        <v>7500.0001124999999</v>
+      </c>
+      <c r="J5">
+        <f>$J$3*D5*B5</f>
+        <v>2142.8571750000001</v>
+      </c>
+      <c r="K5">
+        <f>$K$3*D5*B5</f>
+        <v>10714.285875</v>
+      </c>
+      <c r="L5">
+        <f>$L$3*D5*B5</f>
         <v>8571.4287000000004</v>
       </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I8" si="1">$I$3*D4*B4</f>
-        <v>12857.143050000001</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J8" si="2">$J$3*D4*B4</f>
-        <v>7500.0001124999999</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K8" si="3">$K$3*D4*B4</f>
-        <v>2142.8571750000001</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L8" si="4">$L$3*D4*B4</f>
-        <v>10714.285875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="C6">
-        <v>5.3</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>0.14285713999999999</v>
@@ -644,35 +631,35 @@
         <v>12</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>$H$3*D6*B6</f>
+        <v>2474.9999505000001</v>
+      </c>
+      <c r="I6">
+        <f>$I$3*D6*B6</f>
+        <v>3849.9999229999999</v>
+      </c>
+      <c r="J6">
+        <f>$J$3*D6*B6</f>
+        <v>1099.9999780000001</v>
+      </c>
+      <c r="K6">
+        <f>$K$3*D6*B6</f>
+        <v>5499.9998899999991</v>
+      </c>
+      <c r="L6">
+        <f>$L$3*D6*B6</f>
         <v>4399.9999120000002</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>6599.9998679999999</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>3849.9999229999999</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>1099.9999780000001</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>5499.9998899999991</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C7">
-        <v>5.9</v>
+        <v>5.3</v>
       </c>
       <c r="D7">
         <v>0.14285713999999999</v>
@@ -681,137 +668,104 @@
         <v>13</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>$H$3*D7*B7</f>
+        <v>2539.2856634999998</v>
+      </c>
+      <c r="I7">
+        <f>$I$3*D7*B7</f>
+        <v>3949.9999209999996</v>
+      </c>
+      <c r="J7">
+        <f>$J$3*D7*B7</f>
+        <v>1128.571406</v>
+      </c>
+      <c r="K7">
+        <f>$K$3*D7*B7</f>
+        <v>5642.8570299999992</v>
+      </c>
+      <c r="L7">
+        <f>$L$3*D7*B7</f>
         <v>4514.2856240000001</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>6771.4284360000001</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>3949.9999209999996</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>1128.571406</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
-        <v>5642.8570299999992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>405</v>
+      </c>
+      <c r="C8">
+        <v>5.9</v>
+      </c>
+      <c r="D8">
+        <v>0.14285713999999999</v>
+      </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>$H$3*D8*B8</f>
+        <v>2603.5713765</v>
+      </c>
+      <c r="I8">
+        <f>$I$3*D8*B8</f>
+        <v>4049.9999189999999</v>
+      </c>
+      <c r="J8">
+        <f>$J$3*D8*B8</f>
+        <v>1157.142834</v>
+      </c>
+      <c r="K8">
+        <f>$K$3*D8*B8</f>
+        <v>5785.7141699999993</v>
+      </c>
+      <c r="L8">
+        <f>$L$3*D8*B8</f>
         <v>4628.571336</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>6942.8570040000004</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>4049.9999189999999</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>1157.142834</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>5785.7141699999993</v>
-      </c>
-      <c r="M8">
-        <f>SUM(H9:L9)</f>
-        <v>148478.571345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+    </row>
+    <row r="9" spans="1:14">
       <c r="G9" t="s">
         <v>15</v>
       </c>
       <c r="H9">
         <f>SUM(H4:H8)</f>
-        <v>30457.14284</v>
+        <v>17132.142847499999</v>
       </c>
       <c r="I9">
         <f>SUM(I4:I8)</f>
-        <v>45685.714260000001</v>
+        <v>26649.999984999995</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9:L9" si="5">SUM(J4:J8)</f>
-        <v>26649.999984999995</v>
+        <f t="shared" ref="J9:L9" si="0">SUM(J4:J8)</f>
+        <v>7614.2857100000001</v>
       </c>
       <c r="K9">
-        <f t="shared" si="5"/>
-        <v>7614.2857100000001</v>
+        <f t="shared" si="0"/>
+        <v>38071.428549999997</v>
       </c>
       <c r="L9">
-        <f t="shared" si="5"/>
-        <v>38071.428549999997</v>
-      </c>
-      <c r="M9">
-        <f>SUM(H10:L10)</f>
-        <v>-1521.428655000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="G10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10">
-        <f>H9-30000</f>
-        <v>457.14284000000043</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ref="I10:L10" si="6">I9-30000</f>
-        <v>15685.714260000001</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="6"/>
-        <v>-3350.0000150000051</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="6"/>
-        <v>-22385.71429</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="6"/>
-        <v>8071.4285499999969</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <f t="shared" si="0"/>
+        <v>30457.14284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="N12">
+        <v>380.71428550000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="C14">
+        <f>B4*D4+B5*D5+B6*D6+B7*D7+B8*D8</f>
+        <v>380.71428549999996</v>
+      </c>
       <c r="H14">
-        <f>H9/L2</f>
-        <v>380.71428550000002</v>
-      </c>
-      <c r="I14">
-        <f>I9/H2</f>
-        <v>380.71428550000002</v>
-      </c>
-      <c r="J14">
-        <f>J9/I2</f>
-        <v>380.7142854999999</v>
-      </c>
-      <c r="K14">
-        <f>K9/J2</f>
-        <v>380.71428550000002</v>
-      </c>
-      <c r="L14">
-        <f>L9/K2</f>
+        <f>H9/H3</f>
         <v>380.71428549999996</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="H15">
-        <f>30000/H14</f>
-        <v>78.799249575309148</v>
-      </c>
-    </row>
+    <row r="23" ht="30.75" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest changes - almost done
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesho\Documents\cutting_scheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF42B1D-EBCA-477A-8618-0CF4D04E6181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9A9DC4-A422-4F10-8FE9-32180CB69415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6390" windowWidth="16440" windowHeight="28440" xr2:uid="{4898FC76-975B-4242-BB8F-A76D91429865}"/>
+    <workbookView xWindow="28680" yWindow="-6390" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{4898FC76-975B-4242-BB8F-A76D91429865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,10 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5293D0-8D68-4052-9E07-2020BCCAE873}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1265,415 +1266,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6E1641-C5E4-4991-AD4E-7BEC479CD038}">
-  <dimension ref="A1:A80"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
-        <v>12149.285900000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>12482.143050000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>6215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>6376.4284360000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>6537.8570040000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>11784.285900000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <v>12107.143050000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <v>5830</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <v>5981.4284360000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10">
-        <v>6132.8570040000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
-        <v>11419.285900000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12">
-        <v>11732.143050000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13">
-        <v>5445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14">
-        <v>5586.4284360000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15">
-        <v>5727.8570040000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16">
-        <v>11054.285900000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <v>11357.143050000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18">
-        <v>5060</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19">
-        <v>5191.4284360000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20">
-        <v>5322.8570040000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21">
-        <v>10689.285900000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22">
-        <v>10982.143050000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23">
-        <v>4675</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24">
-        <v>4796.4284360000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25">
-        <v>4917.8570040000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26">
-        <v>10324.285900000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27">
-        <v>10607.143050000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28">
-        <v>4290</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29">
-        <v>4401.4284360000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30">
-        <v>4512.8570040000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31">
-        <v>9959.2859000000008</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32">
-        <v>10232.143050000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33">
-        <v>3905</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34">
-        <v>4006.4284360000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35">
-        <v>4107.8570040000004</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36">
-        <v>9594.2859000000008</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37">
-        <v>9857.1430500000006</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38">
-        <v>3520</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39">
-        <v>3611.4284360000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40">
-        <v>3702.857004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41">
-        <v>9229.2859000000008</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42">
-        <v>9482.1430500000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43">
-        <v>3135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44">
-        <v>3216.4284360000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45">
-        <v>3297.857004</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46">
-        <v>8864.2859000000008</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47">
-        <v>9107.1430500000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48">
-        <v>2750</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49">
-        <v>2821.4284360000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50">
-        <v>2892.857004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51">
-        <v>8499.2859000000008</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52">
-        <v>8732.1430500000006</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53">
-        <v>2365</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54">
-        <v>2426.4284360000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55">
-        <v>2487.857004</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56">
-        <v>8134.2858999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57">
-        <v>8357.1430500000006</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59">
-        <v>2031.4284359999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60">
-        <v>2082.857004</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61">
-        <v>7769.2858999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62">
-        <v>7982.1430499999997</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64">
-        <v>1636.4284359999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65">
-        <v>1677.857004</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66">
-        <v>7404.2858999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67">
-        <v>7607.1430499999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69">
-        <v>1241.4284359999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70">
-        <v>1272.857004</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71">
-        <v>7039.2858999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72">
-        <v>7232.1430499999997</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74">
-        <v>846.42843600000003</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75">
-        <v>867.85700399999996</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76">
-        <v>6674.2858999999999</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77">
-        <v>6857.1430499999997</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79">
-        <v>451.42843599999998</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80">
-        <v>462.85700400000002</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>